<commit_message>
Completed set up,maybe dig into change stream more
</commit_message>
<xml_diff>
--- a/pa4_updated/results/results.xlsx
+++ b/pa4_updated/results/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="exp_1" sheetId="1" state="visible" r:id="rId2"/>
@@ -603,7 +603,7 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -712,8 +712,8 @@
   </sheetPr>
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G32" activeCellId="0" sqref="G32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -902,7 +902,7 @@
         <v>32</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>-0.976324081421</v>
+        <v>0.976324081421</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>868.186485767364</v>
@@ -1010,7 +1010,7 @@
         <v>512</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>-1.030921936035</v>
+        <v>1.030921936035</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>446.44455909729</v>
@@ -1064,7 +1064,7 @@
         <v>2048</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>-0.909566879272</v>
+        <v>0.909566879272</v>
       </c>
       <c r="H13" s="0" t="n">
         <v>1386.48302555084</v>
@@ -1091,7 +1091,7 @@
         <v>4096</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>-17.038106918335</v>
+        <v>17.038106918335</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>292.249393463135</v>
@@ -1118,7 +1118,7 @@
         <v>8192</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>-0.862836837769</v>
+        <v>0.862836837769</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>630.001640319824</v>
@@ -1145,7 +1145,7 @@
         <v>16384</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>-1.152753829956</v>
+        <v>1.152753829956</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>522.865784168243</v>

</xml_diff>